<commit_message>
Complete upload file quizz, assignment
</commit_message>
<xml_diff>
--- a/server/uploads/assignment.xlsx
+++ b/server/uploads/assignment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nam4\KLTN\Project_ELearning_KLTN\server\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129C6E84-9474-49D4-B10B-A1D2FCD6E594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D67942D-60EC-404E-903F-894B58720428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -424,21 +424,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="21.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,7 +458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -478,7 +478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -498,7 +498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -518,7 +518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -538,7 +538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -558,7 +558,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -598,7 +598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -638,7 +638,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -646,7 +646,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -654,7 +654,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>

</xml_diff>